<commit_message>
fix hardcoded lookup range for AdmitScore, AdmitPain
</commit_message>
<xml_diff>
--- a/models/2025/01 Example Excel Book.xlsx
+++ b/models/2025/01 Example Excel Book.xlsx
@@ -15,6 +15,11 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataChecksum="st+l2OxbEuXr71AL8PFIogOWGsQAoKmNSMEKeuZe3IM="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -871,7 +876,7 @@
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B2, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C2, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D2, AdmitScore!A$2:T$102, Q$1, FALSE) + VLOOKUP(E2, AdmitPain!A$2:T$12, Q$1, FALSE) + VLOOKUP(F2, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G2, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H2, Duration!A$2:V$9, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B2, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C2, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D2, AdmitScore!A$2:T$102, Q$1, FALSE) + VLOOKUP(E2, AdmitPain!A$2:T$12, Q$1, FALSE) + VLOOKUP(F2, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G2, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H2, Duration!A$2:V$9, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B2, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C2, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D2, AdmitScore!A$2:T$102, Q$1, FALSE) + VLOOKUP(E2, AdmitPain!A$2:T$12, Q$1, FALSE) + VLOOKUP(F2, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G2, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H2, Duration!A$2:V$9, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B2, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C2, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D2, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E2, AdmitPain!A$2:T$12, Q$1, FALSE) + VLOOKUP(F2, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G2, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H2, Duration!A$2:V$9, Q$1+2, TRUE) ))</f>
         <v>0.9180908621</v>
       </c>
       <c r="M2" s="2">
@@ -928,7 +933,7 @@
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B3, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C3, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D3, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E3, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F3, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G3, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H3, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B3, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C3, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D3, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E3, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F3, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G3, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H3, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B3, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C3, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D3, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E3, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F3, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G3, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H3, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B3, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C3, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D3, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E3, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F3, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G3, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H3, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.5685736318</v>
       </c>
       <c r="M3" s="2">
@@ -983,7 +988,7 @@
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B4, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C4, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D4, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E4, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F4, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G4, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H4, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B4, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C4, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D4, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E4, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F4, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G4, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H4, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B4, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C4, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D4, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E4, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F4, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G4, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H4, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B4, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C4, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D4, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E4, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F4, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G4, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H4, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.4993974903</v>
       </c>
       <c r="M4" s="2">
@@ -1042,7 +1047,7 @@
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B5, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C5, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D5, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E5, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F5, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G5, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H5, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B5, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C5, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D5, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E5, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F5, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G5, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H5, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B5, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C5, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D5, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E5, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F5, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G5, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H5, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B5, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C5, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D5, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E5, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F5, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G5, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H5, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.4191054352</v>
       </c>
       <c r="M5" s="2">
@@ -1101,7 +1106,7 @@
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B6, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C6, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D6, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E6, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F6, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G6, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H6, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B6, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C6, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D6, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E6, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F6, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G6, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H6, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B6, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C6, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D6, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E6, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F6, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G6, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H6, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B6, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C6, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D6, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E6, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F6, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G6, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H6, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.5123816136</v>
       </c>
       <c r="M6" s="2">
@@ -1160,7 +1165,7 @@
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B7, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C7, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D7, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E7, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F7, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G7, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H7, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B7, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C7, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D7, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E7, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F7, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G7, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H7, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B7, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C7, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D7, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E7, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F7, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G7, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H7, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B7, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C7, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D7, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E7, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F7, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G7, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H7, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.6911986818</v>
       </c>
       <c r="M7" s="2">
@@ -1219,7 +1224,7 @@
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="3">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B8, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C8, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D8, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E8, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F8, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G8, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H8, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B8, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C8, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D8, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E8, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F8, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G8, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H8, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B8, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C8, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D8, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E8, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F8, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G8, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H8, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B8, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C8, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D8, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E8, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F8, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G8, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H8, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.7219077678</v>
       </c>
       <c r="M8" s="4">
@@ -1278,7 +1283,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B9, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C9, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D9, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E9, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F9, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G9, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H9, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B9, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C9, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D9, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E9, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F9, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G9, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H9, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B9, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C9, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D9, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E9, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F9, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G9, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H9, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B9, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C9, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D9, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E9, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F9, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G9, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H9, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.6872062029</v>
       </c>
       <c r="M9" s="2">
@@ -1337,7 +1342,7 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B10, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C10, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D10, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E10, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F10, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G10, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H10, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B10, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C10, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D10, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E10, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F10, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G10, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H10, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B10, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C10, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D10, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E10, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F10, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G10, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H10, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B10, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C10, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D10, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E10, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F10, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G10, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H10, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.7751654863</v>
       </c>
       <c r="M10" s="2">
@@ -1396,7 +1401,7 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B11, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C11, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D11, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E11, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F11, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G11, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H11, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B11, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C11, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D11, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E11, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F11, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G11, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H11, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B11, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C11, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D11, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E11, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F11, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G11, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H11, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B11, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C11, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D11, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E11, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F11, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G11, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H11, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.7985003987</v>
       </c>
       <c r="M11" s="2">
@@ -1455,7 +1460,7 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B12, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C12, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D12, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E12, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F12, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G12, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H12, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B12, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C12, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D12, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E12, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F12, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G12, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H12, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B12, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C12, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D12, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E12, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F12, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G12, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H12, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B12, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C12, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D12, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E12, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F12, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G12, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H12, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.85042734</v>
       </c>
       <c r="M12" s="2">
@@ -1514,7 +1519,7 @@
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B13, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C13, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D13, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E13, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F13, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G13, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H13, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B13, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C13, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D13, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E13, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F13, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G13, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H13, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B13, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C13, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D13, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E13, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F13, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G13, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H13, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B13, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C13, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D13, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E13, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F13, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G13, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H13, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8295945264</v>
       </c>
       <c r="M13" s="2">
@@ -1573,7 +1578,7 @@
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B14, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C14, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D14, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E14, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F14, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G14, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H14, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B14, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C14, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D14, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E14, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F14, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G14, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H14, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B14, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C14, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D14, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E14, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F14, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G14, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H14, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B14, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C14, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D14, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E14, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F14, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G14, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H14, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.883510358</v>
       </c>
       <c r="M14" s="2">
@@ -1632,7 +1637,7 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B15, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C15, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D15, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E15, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F15, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G15, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H15, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B15, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C15, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D15, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E15, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F15, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G15, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H15, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B15, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C15, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D15, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E15, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F15, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G15, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H15, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B15, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C15, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D15, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E15, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F15, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G15, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H15, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.9296093053</v>
       </c>
       <c r="M15" s="2">
@@ -1691,7 +1696,7 @@
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B16, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C16, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D16, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E16, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F16, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G16, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H16, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B16, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C16, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D16, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E16, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F16, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G16, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H16, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B16, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C16, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D16, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E16, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F16, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G16, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H16, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B16, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C16, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D16, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E16, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F16, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G16, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H16, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.9386490778</v>
       </c>
       <c r="M16" s="2">
@@ -1750,7 +1755,7 @@
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B17, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C17, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D17, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E17, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F17, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G17, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H17, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B17, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C17, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D17, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E17, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F17, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G17, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H17, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B17, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C17, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D17, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E17, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F17, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G17, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H17, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B17, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C17, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D17, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E17, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F17, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G17, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H17, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.9473697714</v>
       </c>
       <c r="M17" s="2">
@@ -1809,7 +1814,7 @@
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B18, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C18, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D18, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E18, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F18, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G18, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H18, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B18, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C18, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D18, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E18, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F18, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G18, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H18, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B18, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C18, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D18, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E18, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F18, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G18, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H18, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B18, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C18, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D18, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E18, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F18, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G18, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H18, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.9512068486</v>
       </c>
       <c r="M18" s="2">
@@ -1868,7 +1873,7 @@
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B19, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C19, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D19, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E19, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F19, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G19, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H19, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B19, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C19, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D19, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E19, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F19, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G19, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H19, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B19, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C19, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D19, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E19, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F19, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G19, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H19, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B19, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C19, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D19, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E19, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F19, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G19, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H19, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.9718011082</v>
       </c>
       <c r="M19" s="2">
@@ -1927,7 +1932,7 @@
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B20, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C20, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D20, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E20, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F20, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G20, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H20, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B20, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C20, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D20, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E20, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F20, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G20, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H20, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B20, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C20, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D20, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E20, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F20, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G20, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H20, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B20, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C20, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D20, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E20, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F20, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G20, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H20, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.9597759298</v>
       </c>
       <c r="M20" s="2">
@@ -1986,7 +1991,7 @@
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B21, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C21, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D21, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E21, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F21, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G21, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H21, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B21, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C21, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D21, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E21, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F21, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G21, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H21, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B21, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C21, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D21, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E21, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F21, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G21, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H21, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B21, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C21, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D21, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E21, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F21, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G21, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H21, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8316876983</v>
       </c>
       <c r="M21" s="2">
@@ -2045,7 +2050,7 @@
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B22, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C22, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D22, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E22, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F22, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G22, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H22, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B22, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C22, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D22, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E22, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F22, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G22, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H22, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B22, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C22, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D22, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E22, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F22, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G22, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H22, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B22, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C22, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D22, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E22, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F22, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G22, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H22, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8342500714</v>
       </c>
       <c r="M22" s="2">
@@ -2104,7 +2109,7 @@
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B23, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C23, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D23, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E23, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F23, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G23, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H23, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B23, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C23, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D23, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E23, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F23, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G23, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H23, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B23, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C23, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D23, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E23, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F23, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G23, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H23, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B23, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C23, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D23, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E23, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F23, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G23, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H23, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8579739461</v>
       </c>
       <c r="M23" s="2">
@@ -2159,7 +2164,7 @@
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B24, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C24, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D24, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E24, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F24, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G24, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H24, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B24, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C24, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D24, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E24, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F24, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G24, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H24, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B24, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C24, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D24, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E24, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F24, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G24, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H24, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B24, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C24, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D24, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E24, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F24, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G24, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H24, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8618747398</v>
       </c>
       <c r="M24" s="2">
@@ -2214,7 +2219,7 @@
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B25, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C25, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D25, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E25, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F25, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G25, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H25, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B25, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C25, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D25, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E25, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F25, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G25, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H25, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B25, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C25, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D25, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E25, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F25, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G25, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H25, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B25, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C25, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D25, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E25, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F25, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G25, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H25, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8554110173</v>
       </c>
       <c r="M25" s="2">
@@ -2269,7 +2274,7 @@
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B26, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C26, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D26, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E26, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F26, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G26, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H26, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B26, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C26, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D26, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E26, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F26, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G26, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H26, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B26, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C26, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D26, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E26, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F26, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G26, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H26, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B26, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C26, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D26, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E26, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F26, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G26, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H26, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8694511461</v>
       </c>
       <c r="M26" s="2">

</xml_diff>

<commit_message>
resubmit changes to workbook
</commit_message>
<xml_diff>
--- a/models/2025/01 Example Excel Book.xlsx
+++ b/models/2025/01 Example Excel Book.xlsx
@@ -785,7 +785,6 @@
     <col customWidth="1" min="9" max="9" width="18.0"/>
     <col customWidth="1" min="10" max="10" width="18.63"/>
     <col customWidth="1" min="11" max="11" width="7.63"/>
-    <col customWidth="1" min="12" max="12" width="12.63"/>
     <col customWidth="1" min="13" max="15" width="21.88"/>
     <col customWidth="1" min="16" max="16" width="33.38"/>
     <col customWidth="1" min="17" max="18" width="7.63"/>
@@ -876,7 +875,7 @@
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B2, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C2, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D2, AdmitScore!A$2:T$102, Q$1, FALSE) + VLOOKUP(E2, AdmitPain!A$2:T$12, Q$1, FALSE) + VLOOKUP(F2, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G2, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H2, Duration!A$2:V$9, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B2, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C2, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D2, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E2, AdmitPain!A$2:T$12, Q$1, FALSE) + VLOOKUP(F2, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G2, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H2, Duration!A$2:V$9, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B2, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C2, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D2, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E2, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F2, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G2, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H2, Duration!A$2:V$9, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B2, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C2, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D2, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E2, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F2, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G2, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H2, Duration!A$2:V$9, Q$1+2, TRUE) ))</f>
         <v>0.9180908621</v>
       </c>
       <c r="M2" s="2">
@@ -933,7 +932,7 @@
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B3, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C3, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D3, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E3, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F3, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G3, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H3, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B3, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C3, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D3, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E3, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F3, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G3, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H3, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B3, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C3, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D3, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E3, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F3, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G3, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H3, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B3, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C3, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D3, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E3, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F3, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G3, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H3, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.5685736318</v>
       </c>
       <c r="M3" s="2">
@@ -988,7 +987,7 @@
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B4, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C4, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D4, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E4, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F4, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G4, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H4, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B4, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C4, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D4, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E4, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F4, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G4, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H4, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B4, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C4, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D4, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E4, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F4, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G4, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H4, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B4, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C4, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D4, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E4, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F4, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G4, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H4, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.4993974903</v>
       </c>
       <c r="M4" s="2">
@@ -1047,7 +1046,7 @@
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B5, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C5, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D5, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E5, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F5, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G5, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H5, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B5, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C5, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D5, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E5, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F5, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G5, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H5, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B5, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C5, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D5, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E5, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F5, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G5, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H5, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B5, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C5, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D5, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E5, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F5, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G5, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H5, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.4191054352</v>
       </c>
       <c r="M5" s="2">
@@ -1106,7 +1105,7 @@
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B6, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C6, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D6, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E6, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F6, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G6, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H6, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B6, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C6, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D6, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E6, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F6, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G6, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H6, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B6, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C6, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D6, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E6, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F6, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G6, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H6, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B6, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C6, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D6, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E6, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F6, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G6, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H6, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.5123816136</v>
       </c>
       <c r="M6" s="2">
@@ -1165,7 +1164,7 @@
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B7, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C7, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D7, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E7, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F7, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G7, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H7, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B7, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C7, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D7, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E7, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F7, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G7, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H7, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B7, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C7, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D7, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E7, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F7, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G7, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H7, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B7, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C7, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D7, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E7, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F7, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G7, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H7, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.6911986818</v>
       </c>
       <c r="M7" s="2">
@@ -1224,7 +1223,7 @@
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="3">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B8, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C8, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D8, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E8, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F8, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G8, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H8, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B8, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C8, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D8, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E8, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F8, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G8, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H8, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B8, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C8, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D8, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E8, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F8, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G8, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H8, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B8, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C8, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D8, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E8, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F8, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G8, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H8, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.7219077678</v>
       </c>
       <c r="M8" s="4">
@@ -1283,7 +1282,7 @@
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B9, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C9, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D9, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E9, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F9, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G9, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H9, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B9, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C9, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D9, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E9, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F9, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G9, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H9, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B9, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C9, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D9, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E9, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F9, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G9, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H9, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B9, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C9, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D9, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E9, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F9, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G9, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H9, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.6872062029</v>
       </c>
       <c r="M9" s="2">
@@ -1342,7 +1341,7 @@
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B10, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C10, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D10, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E10, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F10, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G10, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H10, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B10, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C10, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D10, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E10, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F10, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G10, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H10, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B10, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C10, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D10, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E10, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F10, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G10, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H10, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B10, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C10, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D10, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E10, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F10, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G10, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H10, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.7751654863</v>
       </c>
       <c r="M10" s="2">
@@ -1401,7 +1400,7 @@
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B11, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C11, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D11, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E11, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F11, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G11, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H11, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B11, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C11, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D11, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E11, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F11, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G11, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H11, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B11, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C11, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D11, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E11, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F11, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G11, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H11, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B11, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C11, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D11, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E11, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F11, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G11, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H11, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.7985003987</v>
       </c>
       <c r="M11" s="2">
@@ -1460,7 +1459,7 @@
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B12, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C12, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D12, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E12, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F12, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G12, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H12, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B12, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C12, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D12, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E12, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F12, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G12, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H12, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B12, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C12, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D12, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E12, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F12, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G12, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H12, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B12, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C12, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D12, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E12, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F12, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G12, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H12, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.85042734</v>
       </c>
       <c r="M12" s="2">
@@ -1519,7 +1518,7 @@
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B13, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C13, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D13, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E13, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F13, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G13, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H13, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B13, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C13, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D13, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E13, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F13, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G13, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H13, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B13, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C13, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D13, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E13, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F13, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G13, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H13, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B13, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C13, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D13, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E13, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F13, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G13, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H13, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8295945264</v>
       </c>
       <c r="M13" s="2">
@@ -1578,7 +1577,7 @@
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B14, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C14, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D14, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E14, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F14, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G14, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H14, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B14, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C14, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D14, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E14, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F14, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G14, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H14, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B14, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C14, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D14, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E14, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F14, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G14, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H14, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B14, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C14, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D14, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E14, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F14, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G14, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H14, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.883510358</v>
       </c>
       <c r="M14" s="2">
@@ -1637,7 +1636,7 @@
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B15, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C15, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D15, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E15, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F15, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G15, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H15, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B15, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C15, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D15, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E15, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F15, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G15, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H15, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B15, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C15, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D15, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E15, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F15, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G15, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H15, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B15, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C15, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D15, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E15, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F15, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G15, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H15, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.9296093053</v>
       </c>
       <c r="M15" s="2">
@@ -1696,7 +1695,7 @@
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B16, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C16, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D16, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E16, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F16, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G16, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H16, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B16, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C16, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D16, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E16, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F16, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G16, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H16, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B16, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C16, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D16, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E16, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F16, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G16, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H16, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B16, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C16, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D16, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E16, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F16, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G16, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H16, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.9386490778</v>
       </c>
       <c r="M16" s="2">
@@ -1755,7 +1754,7 @@
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B17, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C17, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D17, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E17, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F17, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G17, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H17, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B17, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C17, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D17, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E17, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F17, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G17, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H17, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B17, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C17, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D17, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E17, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F17, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G17, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H17, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B17, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C17, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D17, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E17, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F17, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G17, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H17, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.9473697714</v>
       </c>
       <c r="M17" s="2">
@@ -1814,7 +1813,7 @@
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B18, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C18, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D18, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E18, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F18, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G18, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H18, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B18, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C18, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D18, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E18, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F18, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G18, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H18, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B18, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C18, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D18, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E18, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F18, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G18, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H18, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B18, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C18, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D18, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E18, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F18, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G18, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H18, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.9512068486</v>
       </c>
       <c r="M18" s="2">
@@ -1873,7 +1872,7 @@
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B19, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C19, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D19, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E19, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F19, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G19, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H19, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B19, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C19, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D19, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E19, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F19, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G19, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H19, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B19, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C19, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D19, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E19, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F19, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G19, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H19, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B19, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C19, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D19, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E19, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F19, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G19, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H19, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.9718011082</v>
       </c>
       <c r="M19" s="2">
@@ -1932,7 +1931,7 @@
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B20, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C20, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D20, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E20, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F20, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G20, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H20, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B20, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C20, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D20, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E20, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F20, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G20, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H20, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B20, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C20, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D20, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E20, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F20, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G20, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H20, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B20, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C20, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D20, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E20, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F20, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G20, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H20, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.9597759298</v>
       </c>
       <c r="M20" s="2">
@@ -1991,7 +1990,7 @@
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B21, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C21, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D21, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E21, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F21, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G21, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H21, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B21, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C21, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D21, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E21, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F21, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G21, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H21, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B21, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C21, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D21, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E21, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F21, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G21, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H21, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B21, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C21, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D21, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E21, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F21, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G21, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H21, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8316876983</v>
       </c>
       <c r="M21" s="2">
@@ -2050,7 +2049,7 @@
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B22, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C22, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D22, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E22, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F22, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G22, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H22, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B22, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C22, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D22, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E22, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F22, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G22, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H22, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B22, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C22, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D22, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E22, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F22, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G22, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H22, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B22, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C22, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D22, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E22, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F22, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G22, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H22, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8342500714</v>
       </c>
       <c r="M22" s="2">
@@ -2109,7 +2108,7 @@
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B23, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C23, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D23, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E23, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F23, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G23, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H23, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B23, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C23, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D23, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E23, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F23, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G23, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H23, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B23, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C23, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D23, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E23, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F23, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G23, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H23, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B23, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C23, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D23, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E23, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F23, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G23, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H23, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8579739461</v>
       </c>
       <c r="M23" s="2">
@@ -2164,7 +2163,7 @@
       </c>
       <c r="K24" s="2"/>
       <c r="L24" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B24, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C24, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D24, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E24, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F24, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G24, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H24, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B24, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C24, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D24, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E24, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F24, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G24, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H24, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B24, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C24, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D24, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E24, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F24, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G24, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H24, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B24, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C24, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D24, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E24, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F24, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G24, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H24, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8618747398</v>
       </c>
       <c r="M24" s="2">
@@ -2219,7 +2218,7 @@
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B25, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C25, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D25, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E25, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F25, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G25, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H25, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B25, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C25, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D25, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E25, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F25, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G25, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H25, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B25, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C25, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D25, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E25, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F25, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G25, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H25, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B25, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C25, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D25, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E25, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F25, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G25, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H25, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8554110173</v>
       </c>
       <c r="M25" s="2">
@@ -2274,7 +2273,7 @@
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="1">
-        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B26, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C26, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D26, AdmitScore!A$3:T$103, Q$1, FALSE) + VLOOKUP(E26, AdmitPain!A$3:T$13, Q$1, FALSE) + VLOOKUP(F26, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G26, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H26, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B26, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C26, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D26, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E26, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F26, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G26, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H26, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
+        <f>EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B26, Age!A$13:T$103, Q$1, FALSE) + VLOOKUP(C26, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D26, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E26, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F26, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G26, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H26, Duration!A$2:V$6, Q$1+2, TRUE) )/(1+EXP( VLOOKUP(1, Intercepts!A$2:T$2, Q$1, FALSE) + VLOOKUP(B26, Age!A$2:T$103, Q$1, FALSE) + VLOOKUP(C26, Sex!A$2:T$4, Q$1, FALSE) + VLOOKUP(D26, AdmitScore!A$2:T$103, Q$1, FALSE) + VLOOKUP(E26, AdmitPain!A$2:T$13, Q$1, FALSE) + VLOOKUP(F26, Payer!A$2:T$8, Q$1, FALSE) + VLOOKUP(G26, TxType!A$2:T$3, Q$1, FALSE) + VLOOKUP('Patient Data'!H26, Duration!A$2:V$6, Q$1+2, TRUE) ))</f>
         <v>0.8694511461</v>
       </c>
       <c r="M26" s="2">
@@ -31038,7 +31037,6 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="9.5"/>
     <col customWidth="1" min="2" max="2" width="12.5"/>
-    <col customWidth="1" min="3" max="3" width="12.63"/>
     <col customWidth="1" min="4" max="4" width="17.5"/>
     <col customWidth="1" min="5" max="5" width="12.25"/>
     <col customWidth="1" min="6" max="6" width="25.13"/>
@@ -33837,7 +33835,6 @@
     <col customWidth="1" min="4" max="4" width="13.13"/>
     <col customWidth="1" min="5" max="5" width="12.25"/>
     <col customWidth="1" min="6" max="6" width="14.13"/>
-    <col customWidth="1" min="7" max="7" width="12.63"/>
     <col customWidth="1" min="8" max="8" width="26.0"/>
     <col customWidth="1" min="9" max="9" width="16.88"/>
     <col customWidth="1" min="10" max="12" width="13.13"/>

</xml_diff>

<commit_message>
convert negative values to positive - MSK1 - Promis
</commit_message>
<xml_diff>
--- a/models/2025/01 Example Excel Book.xlsx
+++ b/models/2025/01 Example Excel Book.xlsx
@@ -17,7 +17,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataChecksum="st+l2OxbEuXr71AL8PFIogOWGsQAoKmNSMEKeuZe3IM="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataChecksum="NsmO5FKBA6GmQpcxTe5iEVzqQXnDWeGbT+j3eyKlJ3s="/>
     </ext>
   </extLst>
 </workbook>
@@ -20644,8 +20644,8 @@
         <v>0.033957</v>
       </c>
       <c r="C4" s="9">
-        <f t="shared" ref="C4:C103" si="2">-0.0996*A4</f>
-        <v>-0.0996</v>
+        <f t="shared" ref="C4:C103" si="2">0.0996*A4</f>
+        <v>0.0996</v>
       </c>
       <c r="D4" s="9">
         <f t="shared" ref="D4:D103" si="3">0.038712*A4</f>
@@ -20721,7 +20721,7 @@
       </c>
       <c r="C5" s="9">
         <f t="shared" si="2"/>
-        <v>-0.1992</v>
+        <v>0.1992</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" si="3"/>
@@ -20797,7 +20797,7 @@
       </c>
       <c r="C6" s="9">
         <f t="shared" si="2"/>
-        <v>-0.2988</v>
+        <v>0.2988</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="3"/>
@@ -20873,7 +20873,7 @@
       </c>
       <c r="C7" s="9">
         <f t="shared" si="2"/>
-        <v>-0.3984</v>
+        <v>0.3984</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="3"/>
@@ -20949,7 +20949,7 @@
       </c>
       <c r="C8" s="9">
         <f t="shared" si="2"/>
-        <v>-0.498</v>
+        <v>0.498</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="3"/>
@@ -21025,7 +21025,7 @@
       </c>
       <c r="C9" s="9">
         <f t="shared" si="2"/>
-        <v>-0.5976</v>
+        <v>0.5976</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="3"/>
@@ -21101,7 +21101,7 @@
       </c>
       <c r="C10" s="9">
         <f t="shared" si="2"/>
-        <v>-0.6972</v>
+        <v>0.6972</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" si="3"/>
@@ -21177,7 +21177,7 @@
       </c>
       <c r="C11" s="9">
         <f t="shared" si="2"/>
-        <v>-0.7968</v>
+        <v>0.7968</v>
       </c>
       <c r="D11" s="9">
         <f t="shared" si="3"/>
@@ -21253,7 +21253,7 @@
       </c>
       <c r="C12" s="9">
         <f t="shared" si="2"/>
-        <v>-0.8964</v>
+        <v>0.8964</v>
       </c>
       <c r="D12" s="9">
         <f t="shared" si="3"/>
@@ -21329,7 +21329,7 @@
       </c>
       <c r="C13" s="9">
         <f t="shared" si="2"/>
-        <v>-0.996</v>
+        <v>0.996</v>
       </c>
       <c r="D13" s="9">
         <f t="shared" si="3"/>
@@ -21405,7 +21405,7 @@
       </c>
       <c r="C14" s="9">
         <f t="shared" si="2"/>
-        <v>-1.0956</v>
+        <v>1.0956</v>
       </c>
       <c r="D14" s="9">
         <f t="shared" si="3"/>
@@ -21481,7 +21481,7 @@
       </c>
       <c r="C15" s="9">
         <f t="shared" si="2"/>
-        <v>-1.1952</v>
+        <v>1.1952</v>
       </c>
       <c r="D15" s="9">
         <f t="shared" si="3"/>
@@ -21557,7 +21557,7 @@
       </c>
       <c r="C16" s="9">
         <f t="shared" si="2"/>
-        <v>-1.2948</v>
+        <v>1.2948</v>
       </c>
       <c r="D16" s="9">
         <f t="shared" si="3"/>
@@ -21633,7 +21633,7 @@
       </c>
       <c r="C17" s="9">
         <f t="shared" si="2"/>
-        <v>-1.3944</v>
+        <v>1.3944</v>
       </c>
       <c r="D17" s="9">
         <f t="shared" si="3"/>
@@ -21709,7 +21709,7 @@
       </c>
       <c r="C18" s="9">
         <f t="shared" si="2"/>
-        <v>-1.494</v>
+        <v>1.494</v>
       </c>
       <c r="D18" s="9">
         <f t="shared" si="3"/>
@@ -21785,7 +21785,7 @@
       </c>
       <c r="C19" s="9">
         <f t="shared" si="2"/>
-        <v>-1.5936</v>
+        <v>1.5936</v>
       </c>
       <c r="D19" s="9">
         <f t="shared" si="3"/>
@@ -21861,7 +21861,7 @@
       </c>
       <c r="C20" s="9">
         <f t="shared" si="2"/>
-        <v>-1.6932</v>
+        <v>1.6932</v>
       </c>
       <c r="D20" s="9">
         <f t="shared" si="3"/>
@@ -21937,7 +21937,7 @@
       </c>
       <c r="C21" s="9">
         <f t="shared" si="2"/>
-        <v>-1.7928</v>
+        <v>1.7928</v>
       </c>
       <c r="D21" s="9">
         <f t="shared" si="3"/>
@@ -22013,7 +22013,7 @@
       </c>
       <c r="C22" s="9">
         <f t="shared" si="2"/>
-        <v>-1.8924</v>
+        <v>1.8924</v>
       </c>
       <c r="D22" s="9">
         <f t="shared" si="3"/>
@@ -22089,7 +22089,7 @@
       </c>
       <c r="C23" s="9">
         <f t="shared" si="2"/>
-        <v>-1.992</v>
+        <v>1.992</v>
       </c>
       <c r="D23" s="9">
         <f t="shared" si="3"/>
@@ -22165,7 +22165,7 @@
       </c>
       <c r="C24" s="9">
         <f t="shared" si="2"/>
-        <v>-2.0916</v>
+        <v>2.0916</v>
       </c>
       <c r="D24" s="9">
         <f t="shared" si="3"/>
@@ -22241,7 +22241,7 @@
       </c>
       <c r="C25" s="9">
         <f t="shared" si="2"/>
-        <v>-2.1912</v>
+        <v>2.1912</v>
       </c>
       <c r="D25" s="9">
         <f t="shared" si="3"/>
@@ -22317,7 +22317,7 @@
       </c>
       <c r="C26" s="9">
         <f t="shared" si="2"/>
-        <v>-2.2908</v>
+        <v>2.2908</v>
       </c>
       <c r="D26" s="9">
         <f t="shared" si="3"/>
@@ -22393,7 +22393,7 @@
       </c>
       <c r="C27" s="9">
         <f t="shared" si="2"/>
-        <v>-2.3904</v>
+        <v>2.3904</v>
       </c>
       <c r="D27" s="9">
         <f t="shared" si="3"/>
@@ -22469,7 +22469,7 @@
       </c>
       <c r="C28" s="9">
         <f t="shared" si="2"/>
-        <v>-2.49</v>
+        <v>2.49</v>
       </c>
       <c r="D28" s="9">
         <f t="shared" si="3"/>
@@ -22545,7 +22545,7 @@
       </c>
       <c r="C29" s="9">
         <f t="shared" si="2"/>
-        <v>-2.5896</v>
+        <v>2.5896</v>
       </c>
       <c r="D29" s="9">
         <f t="shared" si="3"/>
@@ -22621,7 +22621,7 @@
       </c>
       <c r="C30" s="9">
         <f t="shared" si="2"/>
-        <v>-2.6892</v>
+        <v>2.6892</v>
       </c>
       <c r="D30" s="9">
         <f t="shared" si="3"/>
@@ -22697,7 +22697,7 @@
       </c>
       <c r="C31" s="9">
         <f t="shared" si="2"/>
-        <v>-2.7888</v>
+        <v>2.7888</v>
       </c>
       <c r="D31" s="9">
         <f t="shared" si="3"/>
@@ -22773,7 +22773,7 @@
       </c>
       <c r="C32" s="9">
         <f t="shared" si="2"/>
-        <v>-2.8884</v>
+        <v>2.8884</v>
       </c>
       <c r="D32" s="9">
         <f t="shared" si="3"/>
@@ -22849,7 +22849,7 @@
       </c>
       <c r="C33" s="9">
         <f t="shared" si="2"/>
-        <v>-2.988</v>
+        <v>2.988</v>
       </c>
       <c r="D33" s="9">
         <f t="shared" si="3"/>
@@ -22925,7 +22925,7 @@
       </c>
       <c r="C34" s="9">
         <f t="shared" si="2"/>
-        <v>-3.0876</v>
+        <v>3.0876</v>
       </c>
       <c r="D34" s="9">
         <f t="shared" si="3"/>
@@ -23001,7 +23001,7 @@
       </c>
       <c r="C35" s="9">
         <f t="shared" si="2"/>
-        <v>-3.1872</v>
+        <v>3.1872</v>
       </c>
       <c r="D35" s="9">
         <f t="shared" si="3"/>
@@ -23077,7 +23077,7 @@
       </c>
       <c r="C36" s="9">
         <f t="shared" si="2"/>
-        <v>-3.2868</v>
+        <v>3.2868</v>
       </c>
       <c r="D36" s="9">
         <f t="shared" si="3"/>
@@ -23153,7 +23153,7 @@
       </c>
       <c r="C37" s="9">
         <f t="shared" si="2"/>
-        <v>-3.3864</v>
+        <v>3.3864</v>
       </c>
       <c r="D37" s="9">
         <f t="shared" si="3"/>
@@ -23229,7 +23229,7 @@
       </c>
       <c r="C38" s="9">
         <f t="shared" si="2"/>
-        <v>-3.486</v>
+        <v>3.486</v>
       </c>
       <c r="D38" s="9">
         <f t="shared" si="3"/>
@@ -23305,7 +23305,7 @@
       </c>
       <c r="C39" s="9">
         <f t="shared" si="2"/>
-        <v>-3.5856</v>
+        <v>3.5856</v>
       </c>
       <c r="D39" s="9">
         <f t="shared" si="3"/>
@@ -23381,7 +23381,7 @@
       </c>
       <c r="C40" s="9">
         <f t="shared" si="2"/>
-        <v>-3.6852</v>
+        <v>3.6852</v>
       </c>
       <c r="D40" s="9">
         <f t="shared" si="3"/>
@@ -23457,7 +23457,7 @@
       </c>
       <c r="C41" s="9">
         <f t="shared" si="2"/>
-        <v>-3.7848</v>
+        <v>3.7848</v>
       </c>
       <c r="D41" s="9">
         <f t="shared" si="3"/>
@@ -23533,7 +23533,7 @@
       </c>
       <c r="C42" s="9">
         <f t="shared" si="2"/>
-        <v>-3.8844</v>
+        <v>3.8844</v>
       </c>
       <c r="D42" s="9">
         <f t="shared" si="3"/>
@@ -23609,7 +23609,7 @@
       </c>
       <c r="C43" s="9">
         <f t="shared" si="2"/>
-        <v>-3.984</v>
+        <v>3.984</v>
       </c>
       <c r="D43" s="9">
         <f t="shared" si="3"/>
@@ -23685,7 +23685,7 @@
       </c>
       <c r="C44" s="9">
         <f t="shared" si="2"/>
-        <v>-4.0836</v>
+        <v>4.0836</v>
       </c>
       <c r="D44" s="9">
         <f t="shared" si="3"/>
@@ -23761,7 +23761,7 @@
       </c>
       <c r="C45" s="9">
         <f t="shared" si="2"/>
-        <v>-4.1832</v>
+        <v>4.1832</v>
       </c>
       <c r="D45" s="9">
         <f t="shared" si="3"/>
@@ -23837,7 +23837,7 @@
       </c>
       <c r="C46" s="9">
         <f t="shared" si="2"/>
-        <v>-4.2828</v>
+        <v>4.2828</v>
       </c>
       <c r="D46" s="9">
         <f t="shared" si="3"/>
@@ -23913,7 +23913,7 @@
       </c>
       <c r="C47" s="9">
         <f t="shared" si="2"/>
-        <v>-4.3824</v>
+        <v>4.3824</v>
       </c>
       <c r="D47" s="9">
         <f t="shared" si="3"/>
@@ -23989,7 +23989,7 @@
       </c>
       <c r="C48" s="9">
         <f t="shared" si="2"/>
-        <v>-4.482</v>
+        <v>4.482</v>
       </c>
       <c r="D48" s="9">
         <f t="shared" si="3"/>
@@ -24065,7 +24065,7 @@
       </c>
       <c r="C49" s="9">
         <f t="shared" si="2"/>
-        <v>-4.5816</v>
+        <v>4.5816</v>
       </c>
       <c r="D49" s="9">
         <f t="shared" si="3"/>
@@ -24141,7 +24141,7 @@
       </c>
       <c r="C50" s="9">
         <f t="shared" si="2"/>
-        <v>-4.6812</v>
+        <v>4.6812</v>
       </c>
       <c r="D50" s="9">
         <f t="shared" si="3"/>
@@ -24217,7 +24217,7 @@
       </c>
       <c r="C51" s="9">
         <f t="shared" si="2"/>
-        <v>-4.7808</v>
+        <v>4.7808</v>
       </c>
       <c r="D51" s="9">
         <f t="shared" si="3"/>
@@ -24293,7 +24293,7 @@
       </c>
       <c r="C52" s="9">
         <f t="shared" si="2"/>
-        <v>-4.8804</v>
+        <v>4.8804</v>
       </c>
       <c r="D52" s="9">
         <f t="shared" si="3"/>
@@ -24369,7 +24369,7 @@
       </c>
       <c r="C53" s="9">
         <f t="shared" si="2"/>
-        <v>-4.98</v>
+        <v>4.98</v>
       </c>
       <c r="D53" s="9">
         <f t="shared" si="3"/>
@@ -24445,7 +24445,7 @@
       </c>
       <c r="C54" s="9">
         <f t="shared" si="2"/>
-        <v>-5.0796</v>
+        <v>5.0796</v>
       </c>
       <c r="D54" s="9">
         <f t="shared" si="3"/>
@@ -24521,7 +24521,7 @@
       </c>
       <c r="C55" s="9">
         <f t="shared" si="2"/>
-        <v>-5.1792</v>
+        <v>5.1792</v>
       </c>
       <c r="D55" s="9">
         <f t="shared" si="3"/>
@@ -24597,7 +24597,7 @@
       </c>
       <c r="C56" s="9">
         <f t="shared" si="2"/>
-        <v>-5.2788</v>
+        <v>5.2788</v>
       </c>
       <c r="D56" s="9">
         <f t="shared" si="3"/>
@@ -24673,7 +24673,7 @@
       </c>
       <c r="C57" s="9">
         <f t="shared" si="2"/>
-        <v>-5.3784</v>
+        <v>5.3784</v>
       </c>
       <c r="D57" s="9">
         <f t="shared" si="3"/>
@@ -24749,7 +24749,7 @@
       </c>
       <c r="C58" s="9">
         <f t="shared" si="2"/>
-        <v>-5.478</v>
+        <v>5.478</v>
       </c>
       <c r="D58" s="9">
         <f t="shared" si="3"/>
@@ -24825,7 +24825,7 @@
       </c>
       <c r="C59" s="9">
         <f t="shared" si="2"/>
-        <v>-5.5776</v>
+        <v>5.5776</v>
       </c>
       <c r="D59" s="9">
         <f t="shared" si="3"/>
@@ -24901,7 +24901,7 @@
       </c>
       <c r="C60" s="9">
         <f t="shared" si="2"/>
-        <v>-5.6772</v>
+        <v>5.6772</v>
       </c>
       <c r="D60" s="9">
         <f t="shared" si="3"/>
@@ -24977,7 +24977,7 @@
       </c>
       <c r="C61" s="9">
         <f t="shared" si="2"/>
-        <v>-5.7768</v>
+        <v>5.7768</v>
       </c>
       <c r="D61" s="9">
         <f t="shared" si="3"/>
@@ -25053,7 +25053,7 @@
       </c>
       <c r="C62" s="9">
         <f t="shared" si="2"/>
-        <v>-5.8764</v>
+        <v>5.8764</v>
       </c>
       <c r="D62" s="9">
         <f t="shared" si="3"/>
@@ -25129,7 +25129,7 @@
       </c>
       <c r="C63" s="9">
         <f t="shared" si="2"/>
-        <v>-5.976</v>
+        <v>5.976</v>
       </c>
       <c r="D63" s="9">
         <f t="shared" si="3"/>
@@ -25205,7 +25205,7 @@
       </c>
       <c r="C64" s="9">
         <f t="shared" si="2"/>
-        <v>-6.0756</v>
+        <v>6.0756</v>
       </c>
       <c r="D64" s="9">
         <f t="shared" si="3"/>
@@ -25281,7 +25281,7 @@
       </c>
       <c r="C65" s="9">
         <f t="shared" si="2"/>
-        <v>-6.1752</v>
+        <v>6.1752</v>
       </c>
       <c r="D65" s="9">
         <f t="shared" si="3"/>
@@ -25357,7 +25357,7 @@
       </c>
       <c r="C66" s="9">
         <f t="shared" si="2"/>
-        <v>-6.2748</v>
+        <v>6.2748</v>
       </c>
       <c r="D66" s="9">
         <f t="shared" si="3"/>
@@ -25433,7 +25433,7 @@
       </c>
       <c r="C67" s="9">
         <f t="shared" si="2"/>
-        <v>-6.3744</v>
+        <v>6.3744</v>
       </c>
       <c r="D67" s="9">
         <f t="shared" si="3"/>
@@ -25509,7 +25509,7 @@
       </c>
       <c r="C68" s="9">
         <f t="shared" si="2"/>
-        <v>-6.474</v>
+        <v>6.474</v>
       </c>
       <c r="D68" s="9">
         <f t="shared" si="3"/>
@@ -25585,7 +25585,7 @@
       </c>
       <c r="C69" s="9">
         <f t="shared" si="2"/>
-        <v>-6.5736</v>
+        <v>6.5736</v>
       </c>
       <c r="D69" s="9">
         <f t="shared" si="3"/>
@@ -25661,7 +25661,7 @@
       </c>
       <c r="C70" s="9">
         <f t="shared" si="2"/>
-        <v>-6.6732</v>
+        <v>6.6732</v>
       </c>
       <c r="D70" s="9">
         <f t="shared" si="3"/>
@@ -25737,7 +25737,7 @@
       </c>
       <c r="C71" s="9">
         <f t="shared" si="2"/>
-        <v>-6.7728</v>
+        <v>6.7728</v>
       </c>
       <c r="D71" s="9">
         <f t="shared" si="3"/>
@@ -25813,7 +25813,7 @@
       </c>
       <c r="C72" s="9">
         <f t="shared" si="2"/>
-        <v>-6.8724</v>
+        <v>6.8724</v>
       </c>
       <c r="D72" s="9">
         <f t="shared" si="3"/>
@@ -25889,7 +25889,7 @@
       </c>
       <c r="C73" s="9">
         <f t="shared" si="2"/>
-        <v>-6.972</v>
+        <v>6.972</v>
       </c>
       <c r="D73" s="9">
         <f t="shared" si="3"/>
@@ -25965,7 +25965,7 @@
       </c>
       <c r="C74" s="9">
         <f t="shared" si="2"/>
-        <v>-7.0716</v>
+        <v>7.0716</v>
       </c>
       <c r="D74" s="9">
         <f t="shared" si="3"/>
@@ -26041,7 +26041,7 @@
       </c>
       <c r="C75" s="9">
         <f t="shared" si="2"/>
-        <v>-7.1712</v>
+        <v>7.1712</v>
       </c>
       <c r="D75" s="9">
         <f t="shared" si="3"/>
@@ -26117,7 +26117,7 @@
       </c>
       <c r="C76" s="9">
         <f t="shared" si="2"/>
-        <v>-7.2708</v>
+        <v>7.2708</v>
       </c>
       <c r="D76" s="9">
         <f t="shared" si="3"/>
@@ -26193,7 +26193,7 @@
       </c>
       <c r="C77" s="9">
         <f t="shared" si="2"/>
-        <v>-7.3704</v>
+        <v>7.3704</v>
       </c>
       <c r="D77" s="9">
         <f t="shared" si="3"/>
@@ -26269,7 +26269,7 @@
       </c>
       <c r="C78" s="9">
         <f t="shared" si="2"/>
-        <v>-7.47</v>
+        <v>7.47</v>
       </c>
       <c r="D78" s="9">
         <f t="shared" si="3"/>
@@ -26345,7 +26345,7 @@
       </c>
       <c r="C79" s="9">
         <f t="shared" si="2"/>
-        <v>-7.5696</v>
+        <v>7.5696</v>
       </c>
       <c r="D79" s="9">
         <f t="shared" si="3"/>
@@ -26421,7 +26421,7 @@
       </c>
       <c r="C80" s="9">
         <f t="shared" si="2"/>
-        <v>-7.6692</v>
+        <v>7.6692</v>
       </c>
       <c r="D80" s="9">
         <f t="shared" si="3"/>
@@ -26497,7 +26497,7 @@
       </c>
       <c r="C81" s="9">
         <f t="shared" si="2"/>
-        <v>-7.7688</v>
+        <v>7.7688</v>
       </c>
       <c r="D81" s="9">
         <f t="shared" si="3"/>
@@ -26573,7 +26573,7 @@
       </c>
       <c r="C82" s="9">
         <f t="shared" si="2"/>
-        <v>-7.8684</v>
+        <v>7.8684</v>
       </c>
       <c r="D82" s="9">
         <f t="shared" si="3"/>
@@ -26649,7 +26649,7 @@
       </c>
       <c r="C83" s="9">
         <f t="shared" si="2"/>
-        <v>-7.968</v>
+        <v>7.968</v>
       </c>
       <c r="D83" s="9">
         <f t="shared" si="3"/>
@@ -26725,7 +26725,7 @@
       </c>
       <c r="C84" s="9">
         <f t="shared" si="2"/>
-        <v>-8.0676</v>
+        <v>8.0676</v>
       </c>
       <c r="D84" s="9">
         <f t="shared" si="3"/>
@@ -26801,7 +26801,7 @@
       </c>
       <c r="C85" s="9">
         <f t="shared" si="2"/>
-        <v>-8.1672</v>
+        <v>8.1672</v>
       </c>
       <c r="D85" s="9">
         <f t="shared" si="3"/>
@@ -26877,7 +26877,7 @@
       </c>
       <c r="C86" s="9">
         <f t="shared" si="2"/>
-        <v>-8.2668</v>
+        <v>8.2668</v>
       </c>
       <c r="D86" s="9">
         <f t="shared" si="3"/>
@@ -26953,7 +26953,7 @@
       </c>
       <c r="C87" s="9">
         <f t="shared" si="2"/>
-        <v>-8.3664</v>
+        <v>8.3664</v>
       </c>
       <c r="D87" s="9">
         <f t="shared" si="3"/>
@@ -27029,7 +27029,7 @@
       </c>
       <c r="C88" s="9">
         <f t="shared" si="2"/>
-        <v>-8.466</v>
+        <v>8.466</v>
       </c>
       <c r="D88" s="9">
         <f t="shared" si="3"/>
@@ -27105,7 +27105,7 @@
       </c>
       <c r="C89" s="9">
         <f t="shared" si="2"/>
-        <v>-8.5656</v>
+        <v>8.5656</v>
       </c>
       <c r="D89" s="9">
         <f t="shared" si="3"/>
@@ -27181,7 +27181,7 @@
       </c>
       <c r="C90" s="9">
         <f t="shared" si="2"/>
-        <v>-8.6652</v>
+        <v>8.6652</v>
       </c>
       <c r="D90" s="9">
         <f t="shared" si="3"/>
@@ -27257,7 +27257,7 @@
       </c>
       <c r="C91" s="9">
         <f t="shared" si="2"/>
-        <v>-8.7648</v>
+        <v>8.7648</v>
       </c>
       <c r="D91" s="9">
         <f t="shared" si="3"/>
@@ -27333,7 +27333,7 @@
       </c>
       <c r="C92" s="9">
         <f t="shared" si="2"/>
-        <v>-8.8644</v>
+        <v>8.8644</v>
       </c>
       <c r="D92" s="9">
         <f t="shared" si="3"/>
@@ -27409,7 +27409,7 @@
       </c>
       <c r="C93" s="9">
         <f t="shared" si="2"/>
-        <v>-8.964</v>
+        <v>8.964</v>
       </c>
       <c r="D93" s="9">
         <f t="shared" si="3"/>
@@ -27485,7 +27485,7 @@
       </c>
       <c r="C94" s="9">
         <f t="shared" si="2"/>
-        <v>-9.0636</v>
+        <v>9.0636</v>
       </c>
       <c r="D94" s="9">
         <f t="shared" si="3"/>
@@ -27561,7 +27561,7 @@
       </c>
       <c r="C95" s="9">
         <f t="shared" si="2"/>
-        <v>-9.1632</v>
+        <v>9.1632</v>
       </c>
       <c r="D95" s="9">
         <f t="shared" si="3"/>
@@ -27637,7 +27637,7 @@
       </c>
       <c r="C96" s="9">
         <f t="shared" si="2"/>
-        <v>-9.2628</v>
+        <v>9.2628</v>
       </c>
       <c r="D96" s="9">
         <f t="shared" si="3"/>
@@ -27713,7 +27713,7 @@
       </c>
       <c r="C97" s="9">
         <f t="shared" si="2"/>
-        <v>-9.3624</v>
+        <v>9.3624</v>
       </c>
       <c r="D97" s="9">
         <f t="shared" si="3"/>
@@ -27789,7 +27789,7 @@
       </c>
       <c r="C98" s="9">
         <f t="shared" si="2"/>
-        <v>-9.462</v>
+        <v>9.462</v>
       </c>
       <c r="D98" s="9">
         <f t="shared" si="3"/>
@@ -27865,7 +27865,7 @@
       </c>
       <c r="C99" s="9">
         <f t="shared" si="2"/>
-        <v>-9.5616</v>
+        <v>9.5616</v>
       </c>
       <c r="D99" s="9">
         <f t="shared" si="3"/>
@@ -27941,7 +27941,7 @@
       </c>
       <c r="C100" s="9">
         <f t="shared" si="2"/>
-        <v>-9.6612</v>
+        <v>9.6612</v>
       </c>
       <c r="D100" s="9">
         <f t="shared" si="3"/>
@@ -28017,7 +28017,7 @@
       </c>
       <c r="C101" s="9">
         <f t="shared" si="2"/>
-        <v>-9.7608</v>
+        <v>9.7608</v>
       </c>
       <c r="D101" s="9">
         <f t="shared" si="3"/>
@@ -28093,7 +28093,7 @@
       </c>
       <c r="C102" s="9">
         <f t="shared" si="2"/>
-        <v>-9.8604</v>
+        <v>9.8604</v>
       </c>
       <c r="D102" s="9">
         <f t="shared" si="3"/>
@@ -28169,7 +28169,7 @@
       </c>
       <c r="C103" s="9">
         <f t="shared" si="2"/>
-        <v>-9.96</v>
+        <v>9.96</v>
       </c>
       <c r="D103" s="9">
         <f t="shared" si="3"/>

</xml_diff>